<commit_message>
Implement distance calculation function
- distance.py
- calculate radial distance from user static input
</commit_message>
<xml_diff>
--- a/Dataset/DES contact list.xlsx
+++ b/Dataset/DES contact list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/supaweemindr/Desktop/DES-Able/Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/supaweemindr/Desktop/IE-Dev/DES-Able32/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF6F6C3-E067-BA49-931C-783FF45828DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A56F7F2-8C0A-3B4F-8E59-15CCAA3E26D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{806FE980-10E9-2D4C-BFB5-8726324C3628}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{806FE980-10E9-2D4C-BFB5-8726324C3628}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>DVJS Employment Solutions</t>
   </si>
   <si>
-    <t>Dandenong</t>
-  </si>
-  <si>
     <t>Cranbourne</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>cranbourne@echoaustralia.com</t>
   </si>
   <si>
-    <t>dandenong@echoaustralia.com</t>
-  </si>
-  <si>
     <t>Greensborough</t>
   </si>
   <si>
@@ -236,9 +230,6 @@
     <t>MAX Employment</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>OCTEC</t>
   </si>
   <si>
@@ -471,6 +462,15 @@
   </si>
   <si>
     <t>enquiriesVIC@signforwork.org.au</t>
+  </si>
+  <si>
+    <t>DandeNot available ng</t>
+  </si>
+  <si>
+    <t>dandeNot available ng@echoaustralia.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available </t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B143412D-2DDD-0B40-B5D7-D17D3C0DE430}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -955,7 +955,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>4</v>
@@ -964,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -978,12 +978,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -1132,12 +1132,12 @@
         <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
@@ -1160,7 +1160,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -1174,7 +1174,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -1182,13 +1182,13 @@
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -1196,13 +1196,13 @@
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -1210,13 +1210,13 @@
         <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -1224,13 +1224,13 @@
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
@@ -1238,13 +1238,13 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -1252,13 +1252,13 @@
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -1266,388 +1266,388 @@
         <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D33" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>13</v>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="51" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>9</v>
@@ -1669,13 +1669,13 @@
     </row>
     <row r="52" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B52" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>14</v>
@@ -1683,83 +1683,83 @@
     </row>
     <row r="53" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>7</v>
@@ -1767,27 +1767,27 @@
     </row>
     <row r="59" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>16</v>
@@ -1795,27 +1795,27 @@
     </row>
     <row r="61" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>22</v>
@@ -1823,27 +1823,27 @@
     </row>
     <row r="63" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>20</v>
@@ -1851,13 +1851,13 @@
     </row>
     <row r="65" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
@@ -1865,13 +1865,13 @@
     </row>
     <row r="66" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>18</v>
@@ -1879,86 +1879,86 @@
     </row>
     <row r="67" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="14" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1977,7 +1977,7 @@
     <hyperlink ref="B16" r:id="rId12" xr:uid="{73771616-5395-8147-992D-BB821AD9F4A5}"/>
     <hyperlink ref="C16" r:id="rId13" display="mailto:hello@campbellpage.org.au" xr:uid="{A236B6CA-2984-B249-ADA7-F7AC42A863EC}"/>
     <hyperlink ref="C25" r:id="rId14" display="mailto:cranbourne@echoaustralia.com" xr:uid="{88C0F322-7336-0448-BA36-89AD129AC491}"/>
-    <hyperlink ref="C26" r:id="rId15" xr:uid="{E465D50A-0D44-3A4E-9564-2B513C648F63}"/>
+    <hyperlink ref="C26" r:id="rId15" display="dandenong@echoaustralia.com" xr:uid="{E465D50A-0D44-3A4E-9564-2B513C648F63}"/>
     <hyperlink ref="C27" r:id="rId16" display="mailto:green@echoaustralia.com" xr:uid="{6507FB69-DD8E-544A-960A-9C437F75BDCD}"/>
     <hyperlink ref="C28" r:id="rId17" xr:uid="{EA3A0727-042C-E64C-B1A2-6F9F15FBD655}"/>
     <hyperlink ref="C29" r:id="rId18" display="mailto:narre@echoaustralia.com" xr:uid="{847714EB-0678-CE40-8C0F-E6B0AA8BC04E}"/>

</xml_diff>